<commit_message>
sum up by year
</commit_message>
<xml_diff>
--- a/기업_고용_산업대분류별.xlsx
+++ b/기업_고용_산업대분류별.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,6 +459,16 @@
           <t>중기업_소계_2023</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>2022_종사자수</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>2023_종사자수</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -478,6 +488,12 @@
       <c r="E2" t="n">
         <v>0</v>
       </c>
+      <c r="F2" t="n">
+        <v>67</v>
+      </c>
+      <c r="G2" t="n">
+        <v>113</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -497,6 +513,12 @@
       <c r="E3" t="n">
         <v>0</v>
       </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -516,6 +538,12 @@
       <c r="E4" t="n">
         <v>3870</v>
       </c>
+      <c r="F4" t="n">
+        <v>14377</v>
+      </c>
+      <c r="G4" t="n">
+        <v>14640</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -535,6 +563,12 @@
       <c r="E5" t="n">
         <v>0</v>
       </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -554,6 +588,12 @@
       <c r="E6" t="n">
         <v>422</v>
       </c>
+      <c r="F6" t="n">
+        <v>1545</v>
+      </c>
+      <c r="G6" t="n">
+        <v>539</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -573,6 +613,12 @@
       <c r="E7" t="n">
         <v>7265</v>
       </c>
+      <c r="F7" t="n">
+        <v>13439</v>
+      </c>
+      <c r="G7" t="n">
+        <v>13342</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -592,6 +638,12 @@
       <c r="E8" t="n">
         <v>13402</v>
       </c>
+      <c r="F8" t="n">
+        <v>24862</v>
+      </c>
+      <c r="G8" t="n">
+        <v>24552</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -611,6 +663,12 @@
       <c r="E9" t="n">
         <v>1886</v>
       </c>
+      <c r="F9" t="n">
+        <v>4745</v>
+      </c>
+      <c r="G9" t="n">
+        <v>4139</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -630,6 +688,12 @@
       <c r="E10" t="n">
         <v>4512</v>
       </c>
+      <c r="F10" t="n">
+        <v>8690</v>
+      </c>
+      <c r="G10" t="n">
+        <v>9110</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -649,6 +713,12 @@
       <c r="E11" t="n">
         <v>672</v>
       </c>
+      <c r="F11" t="n">
+        <v>3323</v>
+      </c>
+      <c r="G11" t="n">
+        <v>3329</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -668,6 +738,12 @@
       <c r="E12" t="n">
         <v>0</v>
       </c>
+      <c r="F12" t="n">
+        <v>363</v>
+      </c>
+      <c r="G12" t="n">
+        <v>153</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -687,6 +763,12 @@
       <c r="E13" t="n">
         <v>2885</v>
       </c>
+      <c r="F13" t="n">
+        <v>3821</v>
+      </c>
+      <c r="G13" t="n">
+        <v>4050</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -706,6 +788,12 @@
       <c r="E14" t="n">
         <v>2314</v>
       </c>
+      <c r="F14" t="n">
+        <v>6375</v>
+      </c>
+      <c r="G14" t="n">
+        <v>6603</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -725,6 +813,12 @@
       <c r="E15" t="n">
         <v>9083</v>
       </c>
+      <c r="F15" t="n">
+        <v>12695</v>
+      </c>
+      <c r="G15" t="n">
+        <v>13294</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -744,6 +838,12 @@
       <c r="E16" t="n">
         <v>870</v>
       </c>
+      <c r="F16" t="n">
+        <v>1622</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1639</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -763,6 +863,12 @@
       <c r="E17" t="n">
         <v>8867</v>
       </c>
+      <c r="F17" t="n">
+        <v>10048</v>
+      </c>
+      <c r="G17" t="n">
+        <v>10966</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -782,6 +888,12 @@
       <c r="E18" t="n">
         <v>712</v>
       </c>
+      <c r="F18" t="n">
+        <v>1678</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1699</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -801,6 +913,12 @@
       <c r="E19" t="n">
         <v>2036</v>
       </c>
+      <c r="F19" t="n">
+        <v>3104</v>
+      </c>
+      <c r="G19" t="n">
+        <v>3084</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -819,6 +937,12 @@
       </c>
       <c r="E20" t="n">
         <v>60024</v>
+      </c>
+      <c r="F20" t="n">
+        <v>75307</v>
+      </c>
+      <c r="G20" t="n">
+        <v>112962</v>
       </c>
     </row>
   </sheetData>

</xml_diff>